<commit_message>
FCT feed start concentration
</commit_message>
<xml_diff>
--- a/data/FCT/IC_data.xlsx
+++ b/data/FCT/IC_data.xlsx
@@ -8,9 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/FCT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="550" documentId="8_{1BFCB0D7-5E18-453F-9780-0136500C8DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{474EF7A5-77DB-4D31-8942-B496F45F3E61}"/>
+  <xr:revisionPtr revIDLastSave="713" documentId="8_{1BFCB0D7-5E18-453F-9780-0136500C8DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CA4A6AA-F231-4257-A4AC-5110CF076C9C}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3FD8DA9B-E30D-4846-970A-3E60733D34F4}"/>
+    <workbookView visibility="hidden" xWindow="1710" yWindow="3705" windowWidth="21600" windowHeight="11385" activeTab="7" xr2:uid="{3FD8DA9B-E30D-4846-970A-3E60733D34F4}"/>
+    <workbookView xWindow="-645" yWindow="8640" windowWidth="21600" windowHeight="11385" activeTab="7" xr2:uid="{895A1CFC-8652-432C-9303-BF8517F8F540}"/>
   </bookViews>
   <sheets>
     <sheet name="Cl" sheetId="1" r:id="rId1"/>
@@ -20,6 +21,7 @@
     <sheet name="Br" sheetId="5" r:id="rId5"/>
     <sheet name="Mg" sheetId="6" r:id="rId6"/>
     <sheet name="Kalium" sheetId="8" r:id="rId7"/>
+    <sheet name="mM" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="39">
   <si>
     <t>1A</t>
   </si>
@@ -107,6 +109,57 @@
   <si>
     <t xml:space="preserve">Måske der er noget interferens. </t>
   </si>
+  <si>
+    <t>Cl</t>
+  </si>
+  <si>
+    <t>6A</t>
+  </si>
+  <si>
+    <t>6B</t>
+  </si>
+  <si>
+    <t>7A</t>
+  </si>
+  <si>
+    <t>7B</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>mM</t>
+  </si>
+  <si>
+    <t>SO4</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>Br</t>
+  </si>
+  <si>
+    <t>Mg</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Mw</t>
+  </si>
+  <si>
+    <t>dil</t>
+  </si>
+  <si>
+    <t>NaOH</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
 </sst>
 </file>
 
@@ -121,12 +174,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -141,12 +224,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2791,8 +2896,9 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B30"/>
+      <selection activeCell="D24" sqref="D24:F24"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3410,9 +3516,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56731F29-9D56-4977-ABB4-C964ED592116}">
   <dimension ref="A1:AJ30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AJ14" sqref="AJ14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24:F24"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3487,15 +3594,15 @@
         <f t="shared" ref="I3:I30" si="0">AVERAGE(E3:F3)*D3</f>
         <v>71.378500000000003</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2"/>
+      <c r="M3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="6"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="2"/>
+      <c r="P3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="6"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -3774,15 +3881,15 @@
         <f t="shared" si="0"/>
         <v>161.07249999999999</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N10" s="2"/>
+      <c r="N10" s="6"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="2" t="s">
+      <c r="P10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="Q10" s="2"/>
+      <c r="Q10" s="6"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -4422,8 +4529,9 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="D24" sqref="D24:F24"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5041,8 +5149,9 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="D24" sqref="D24:F24"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5660,8 +5769,9 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D24" sqref="D24:F24"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6279,8 +6389,9 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1"/>
+      <selection activeCell="D24" sqref="D24:F24"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6898,8 +7009,9 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D24" sqref="D24:F24"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7510,4 +7622,777 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B4111D8-380E-405F-96EC-1398058A0616}">
+  <dimension ref="A1:V36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="1">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="8" width="9.140625" style="2"/>
+    <col min="12" max="13" width="9.140625" style="2"/>
+    <col min="17" max="18" width="9.140625" style="2"/>
+    <col min="22" max="22" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <v>34.450000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>96.06</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4">
+        <v>40.078000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5">
+        <v>22.98977</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6">
+        <v>79.903999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7">
+        <v>24.305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8">
+        <v>39.098300000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>60.912999999999997</v>
+      </c>
+      <c r="E16">
+        <v>67.331999999999994</v>
+      </c>
+      <c r="F16">
+        <f>AVERAGE((C16*D16),(E16*C16))</f>
+        <v>64.122500000000002</v>
+      </c>
+      <c r="G16" s="2">
+        <f>F16/$E2</f>
+        <v>1.861320754716981</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>17.766999999999999</v>
+      </c>
+      <c r="J16">
+        <v>17.795999999999999</v>
+      </c>
+      <c r="K16">
+        <f>AVERAGE((H16*I16),(J16*H16))</f>
+        <v>88.907499999999999</v>
+      </c>
+      <c r="L16" s="2">
+        <f>K16/$E2</f>
+        <v>2.5807692307692305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>71.382999999999996</v>
+      </c>
+      <c r="E17">
+        <v>71.373999999999995</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ref="F17:F22" si="0">AVERAGE((C17*D17),(E17*C17))</f>
+        <v>71.378500000000003</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" ref="G17:G22" si="1">F17/$E3</f>
+        <v>0.74306162814907351</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17">
+        <v>3.4784000000000002</v>
+      </c>
+      <c r="K17">
+        <v>3.4605999999999999</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" ref="L17:L22" si="2">K17/$E3</f>
+        <v>3.6025400791172182E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>17.440999999999999</v>
+      </c>
+      <c r="E18">
+        <v>17.295000000000002</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>17.368000000000002</v>
+      </c>
+      <c r="G18" s="2">
+        <f>F18/$E4</f>
+        <v>0.43335495783222716</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>3.9790000000000001</v>
+      </c>
+      <c r="J18">
+        <v>4.1829999999999998</v>
+      </c>
+      <c r="K18">
+        <f t="shared" ref="K18:K22" si="3">AVERAGE((H18*I18),(J18*H18))</f>
+        <v>4.0809999999999995</v>
+      </c>
+      <c r="L18" s="2">
+        <f>K18/$E4</f>
+        <v>0.10182643844503217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>(G19/1000)*E5*10</f>
+        <v>3.9816999999999996</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>80.176000000000002</v>
+      </c>
+      <c r="E19">
+        <v>79.091999999999999</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>398.16999999999996</v>
+      </c>
+      <c r="G19" s="2">
+        <f>F19/$E5</f>
+        <v>17.319442517258761</v>
+      </c>
+      <c r="H19">
+        <v>5</v>
+      </c>
+      <c r="I19">
+        <v>41.265000000000001</v>
+      </c>
+      <c r="J19">
+        <v>40.737000000000002</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="3"/>
+        <v>205.005</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="2"/>
+        <v>8.917227097095795</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>2.85</v>
+      </c>
+      <c r="E20">
+        <v>2.8540000000000001</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>2.8520000000000003</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>3.5692831397677219E-2</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>3.286</v>
+      </c>
+      <c r="J20">
+        <v>4.0220000000000002</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="3"/>
+        <v>3.6539999999999999</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="2"/>
+        <v>4.5729875851021229E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>5.7709999999999999</v>
+      </c>
+      <c r="E21">
+        <v>5.6420000000000003</v>
+      </c>
+      <c r="F21">
+        <f>AVERAGE((C21*D21),(E21*C21))</f>
+        <v>5.7065000000000001</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>0.23478708084756225</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1.359</v>
+      </c>
+      <c r="J21">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="K21">
+        <f>AVERAGE((H21*I21),(J21*H21))</f>
+        <v>1.163</v>
+      </c>
+      <c r="L21" s="2">
+        <f>K21/$E7</f>
+        <v>4.7850236576836042E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>6.9130000000000003</v>
+      </c>
+      <c r="E22">
+        <v>5.6189999999999998</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>6.266</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16026272242015638</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>3.8029999999999999</v>
+      </c>
+      <c r="J22">
+        <v>3.11</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="3"/>
+        <v>3.4565000000000001</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="2"/>
+        <v>8.840537823895156E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>C23*E5*0.015</f>
+        <v>1.0345396499999999E-2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23">
+        <f>2*0.015</f>
+        <v>0.03</v>
+      </c>
+      <c r="H23"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f>A19-A23</f>
+        <v>3.9713546034999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C26" s="4"/>
+      <c r="D26" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C27" s="2"/>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="K27" t="s">
+        <v>27</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>45.151000000000003</v>
+      </c>
+      <c r="E28">
+        <v>45.142000000000003</v>
+      </c>
+      <c r="F28">
+        <f t="shared" ref="F28:F34" si="4">AVERAGE((C28*D28),(E28*C28))</f>
+        <v>45.146500000000003</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" ref="G28:G34" si="5">F28/$E2</f>
+        <v>1.3104934687953556</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>56.649000000000001</v>
+      </c>
+      <c r="J28">
+        <v>57.764000000000003</v>
+      </c>
+      <c r="K28">
+        <f>AVERAGE((H28*I28),(J28*H28))</f>
+        <v>57.206500000000005</v>
+      </c>
+      <c r="L28" s="2">
+        <f t="shared" ref="L28:L34" si="6">K28/$E2</f>
+        <v>1.6605660377358491</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>32.185000000000002</v>
+      </c>
+      <c r="E29">
+        <v>32.244</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="4"/>
+        <v>161.07249999999999</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="5"/>
+        <v>1.6767905475744325</v>
+      </c>
+      <c r="H29">
+        <v>5</v>
+      </c>
+      <c r="I29">
+        <v>3.2292000000000001</v>
+      </c>
+      <c r="J29">
+        <v>3.2778999999999998</v>
+      </c>
+      <c r="K29">
+        <f t="shared" ref="K29:K34" si="7">AVERAGE((H29*I29),(J29*H29))</f>
+        <v>16.267749999999999</v>
+      </c>
+      <c r="L29" s="2">
+        <f t="shared" si="6"/>
+        <v>0.16934988548823651</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>17.798999999999999</v>
+      </c>
+      <c r="E30">
+        <v>17.759</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="4"/>
+        <v>17.779</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="5"/>
+        <v>0.44360996057687507</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>5.5919999999999996</v>
+      </c>
+      <c r="J30">
+        <v>5.0620000000000003</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="7"/>
+        <v>5.327</v>
+      </c>
+      <c r="L30" s="2">
+        <f t="shared" si="6"/>
+        <v>0.13291581416238335</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f>(G31/1000)*E5*10</f>
+        <v>2.6602750000000004</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>53.366</v>
+      </c>
+      <c r="E31">
+        <v>53.045000000000002</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="4"/>
+        <v>266.02750000000003</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="5"/>
+        <v>11.571559872064837</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+      <c r="I31">
+        <v>34.161999999999999</v>
+      </c>
+      <c r="J31">
+        <v>33.947000000000003</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="7"/>
+        <v>170.27250000000001</v>
+      </c>
+      <c r="L31" s="2">
+        <f t="shared" si="6"/>
+        <v>7.4064464324784458</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>2.0219999999999998</v>
+      </c>
+      <c r="E32">
+        <v>2.024</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="4"/>
+        <v>2.0229999999999997</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="5"/>
+        <v>2.5317881457749297E-2</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>2.7930000000000001</v>
+      </c>
+      <c r="J32">
+        <v>2.8410000000000002</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="7"/>
+        <v>2.8170000000000002</v>
+      </c>
+      <c r="L32" s="2">
+        <f t="shared" si="6"/>
+        <v>3.5254805766920305E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>31.71</v>
+      </c>
+      <c r="E33">
+        <v>31.765999999999998</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="4"/>
+        <v>31.738</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="5"/>
+        <v>1.3058218473565111</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>2.9260000000000002</v>
+      </c>
+      <c r="J33">
+        <v>3.24</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="7"/>
+        <v>3.0830000000000002</v>
+      </c>
+      <c r="L33" s="2">
+        <f t="shared" si="6"/>
+        <v>0.12684632791606668</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>4.6740000000000004</v>
+      </c>
+      <c r="E34">
+        <v>3.9249999999999998</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="4"/>
+        <v>4.2995000000000001</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="5"/>
+        <v>0.10996641797725221</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>3.2850000000000001</v>
+      </c>
+      <c r="J34">
+        <v>2.7040000000000002</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="7"/>
+        <v>2.9945000000000004</v>
+      </c>
+      <c r="L34" s="2">
+        <f t="shared" si="6"/>
+        <v>7.6589007706217418E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f>C35*E5*0.015</f>
+        <v>7.5866240999999997E-3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35">
+        <f>2*0.011</f>
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f>A31-A35</f>
+        <v>2.6526883759000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="I26:L26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>